<commit_message>
Expanded regression suite with all modules
</commit_message>
<xml_diff>
--- a/data/schemeCategory.xlsx
+++ b/data/schemeCategory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C710DB-76F6-4368-AA93-89D2FB1965B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E2815B-77B6-4302-B9BD-3E12144B39A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet51" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
@@ -43,7 +43,7 @@
     <sheet name="Sheet33" sheetId="33" r:id="rId33"/>
     <sheet name="Sheet34" sheetId="34" r:id="rId34"/>
     <sheet name="Sheet35" sheetId="35" r:id="rId35"/>
-    <sheet name="Sheet36" sheetId="36" r:id="rId36"/>
+    <sheet name="Sheet50" sheetId="36" r:id="rId36"/>
     <sheet name="Sheet37" sheetId="37" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -62,9 +62,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="67">
-  <si>
-    <t>MITCHELLS &amp; BUTLERS PENSION PLAN</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="86">
+  <si>
+    <t>GF61865001 - YOUR SODEXO RETIREMENT PLAN</t>
+  </si>
+  <si>
+    <t>MySI Name/Title</t>
   </si>
   <si>
     <t>Master Data</t>
@@ -73,88 +76,169 @@
     <t>Actual Data</t>
   </si>
   <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
     <t>Result</t>
   </si>
   <si>
+    <t>Table - Scheme Category with Target Retirement Age</t>
+  </si>
+  <si>
+    <t>["Sodexo Ltd - Monthly Paid","65","17,494","Sodexo Ltd - AE Weekly Paid","65","4,005","Sodexo Ltd - AE Monthly Paid","65","342","Sodexo Motivation Solutions UK Ltd","65","216","Sodexo Global Services Ltd","65","82","TVF Weekly Paid","65","21","Sports Travel &amp; Hospitality Group Ltd","65","18","Sodexo Ltd - Four Weekly Paid","65","9","Sodexo Travel","65","0"]</t>
+  </si>
+  <si>
+    <t>Table - AMC Bands by Scheme Category</t>
+  </si>
+  <si>
+    <t>["GF61865001","Sodexo Global Services Ltd","Less than: 50000.0 - 0.19","GF61865001","Sodexo Global Services Ltd","Over: 50000.0 - 0.19","GF61865001","Sodexo Ltd - AE Monthly Paid","Less than: 50000.0 - 0.19","GF61865001","Sodexo Ltd - AE Monthly Paid","Over: 50000.0 - 0.19","GF61865001","Sodexo Ltd - AE Weekly Paid","Less than: 50000.0 - 0.19","GF61865001","Sodexo Ltd - AE Weekly Paid","Over: 50000.0 - 0.19","GF61865001","Sodexo Ltd - Four Weekly Paid","Less than: 50000.0 - 0.19","GF61865001","Sodexo Ltd - Four Weekly Paid","Over: 50000.0 - 0.19","GF61865001","Sodexo Ltd - Monthly Paid","Less than: 50000.0 - 0.19","GF61865001","Sodexo Ltd - Monthly Paid","Over: 50000.0 - 0.19","GF61865001","Sodexo Motivation Solutions UK Ltd","Less than: 50000.0 - 0.19","GF61865001","Sodexo Motivation Solutions UK Ltd","Over: 50000.0 - 0.19","GF61865001","Sodexo Travel","Less than: 50000.0 - 1.19","GF61865001","Sodexo Travel","Over: 50000.0 - 1.19","GF61865001","Sports Travel &amp; Hospitality Group Ltd","Less than: 50000.0 - 0.19","GF61865001","Sports Travel &amp; Hospitality Group Ltd","Over: 50000.0 - 0.19","GF61865001","TVF Four weekly Temporary","Less than: 50000.0 - 1.19","GF61865001","TVF Four weekly Temporary","Over: 50000.0 - 1.19","GF61865001","TVF Weekly Paid","Less than: 50000.0 - 0.19","GF61865001","TVF Weekly Paid","Over: 50000.0 - 0.19"]</t>
+  </si>
+  <si>
+    <t>Table - Scheme Category with Default Investment Strategy</t>
+  </si>
+  <si>
+    <t>["Sodexo Ltd - Monthly Paid","L&amp;G PMC Multi-Asset 3","100","0.13%","Sodexo Ltd - Four Weekly Paid","L&amp;G PMC Multi-Asset 3","100","0.13%","Sodexo Ltd - AE Monthly Paid","L&amp;G PMC Multi-Asset 3","100","0.13%","Sodexo Ltd - AE Weekly Paid","L&amp;G PMC Multi-Asset 3","100","0.13%","TVF Weekly Paid","L&amp;G PMC Multi-Asset 3","100","0.13%","TVF Four weekly Temporary","L&amp;G PMC Multi-Asset 3","100","0.13%","Sodexo Global Services Ltd","L&amp;G PMC Multi-Asset 3","100","0.13%","Sports Travel &amp; Hospitality Group Ltd","L&amp;G PMC Multi-Asset 3","100","0.13%","Sodexo Motivation Solutions UK Ltd","L&amp;G PMC Multi-Asset 3","100","0.13%","Sodexo Travel","L&amp;G PMC Multi-Asset 3","100","0.13%"]</t>
+  </si>
+  <si>
+    <t>Scheme Category Description Filter</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Age Band Filter</t>
+  </si>
+  <si>
+    <t>Filter is displayed</t>
+  </si>
+  <si>
+    <t>Company Name Filter</t>
+  </si>
+  <si>
+    <t>Gender Filter</t>
+  </si>
+  <si>
+    <t>Gone Away Indicator Filter</t>
+  </si>
+  <si>
+    <t>Group Scheme Type Filter</t>
+  </si>
+  <si>
+    <t>Member Status Filter</t>
+  </si>
+  <si>
+    <t>National Insurance No Filter</t>
+  </si>
+  <si>
+    <t>Scheme ID Filter</t>
+  </si>
+  <si>
+    <t>Year/Month Filter</t>
+  </si>
+  <si>
+    <t>Individual values of Table - Scheme Category with Target Retirement Age</t>
+  </si>
+  <si>
+    <t>Sodexo Ltd Monthly Paid - Count Of Policies</t>
+  </si>
+  <si>
+    <t>Sodexo Ltd AE Weekly Paid - Count Of Policies</t>
+  </si>
+  <si>
+    <t>Sodexo Ltd AE Monthly Paid - Count Of Policies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodexo Motivation Solutions UK Ltd               </t>
+  </si>
+  <si>
+    <t>Sodexo Global Services Ltd</t>
+  </si>
+  <si>
+    <t>TVF Weekly Paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports Travel &amp; Hospitality Group Ltd                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodexo Ltd - Four Weekly Paid                               </t>
+  </si>
+  <si>
+    <t>Sodexo Travel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVF Four weekly Temporary                                   </t>
+  </si>
+  <si>
+    <t>SAINSBURY'S RETIREMENT SAVINGS PLAN</t>
+  </si>
+  <si>
+    <t>["GF71965001","Ex Stakeholder &amp; SIPP Members","Less than: 50000.0 - 0.2","GF71965001","Ex Stakeholder &amp; SIPP Members","Over: 50000.0 - 0.2","GF71965001","Income Drawdown Category","Less than: 50000.0 - 0.2","GF71965001","Income Drawdown Category","Over: 50000.0 - 0.2","GF71965001","New Members","Less than: 50000.0 - 0.2","GF71965001","New Members","Over: 50000.0 - 0.2"]</t>
+  </si>
+  <si>
+    <t>["Ex Stakeholder &amp; SIPP Members","L&amp;G PMC 2015 - 2020 Target Date Fund 3","100","0.15%","New Members","L&amp;G PMC 2015 - 2020 Target Date Fund 3","100","0.15%","Income Drawdown Category","L&amp;G PMC 2015 - 2020 Target Date Fund 3","100","0.15%"]</t>
+  </si>
+  <si>
+    <t>New Members</t>
+  </si>
+  <si>
+    <t>Ex stakeholders &amp; SIPP Members</t>
+  </si>
+  <si>
+    <t>Drawdown category</t>
+  </si>
+  <si>
+    <t>THE TESCO RETIREMENT SAVINGS PLAN</t>
+  </si>
+  <si>
     <t>Category selected retirement age heading</t>
   </si>
   <si>
+    <t>8,873</t>
+  </si>
+  <si>
+    <t>Category selected retirement age data</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>["14,594","11,696","3,486","1,560","1,552","0"]</t>
+  </si>
+  <si>
+    <t>["TOTAL CALLS RECEIVED","32,888"]</t>
+  </si>
+  <si>
+    <t>RBS GROUP RETIREMENT SAVINGS PLAN (GIB)</t>
+  </si>
+  <si>
+    <t>SERCO</t>
+  </si>
+  <si>
+    <t>RBS GROUP RETIREMENT SAVINGS PLAN</t>
+  </si>
+  <si>
+    <t>1,884</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>["5,232","1,040","921","724","464","0"]</t>
+  </si>
+  <si>
+    <t>["TOTAL CALLS RECEIVED","8,381"]</t>
+  </si>
+  <si>
+    <t>SIEMENS HEALTHINEERS PENSION PLAN</t>
+  </si>
+  <si>
     <t>["Scheme Category Description","Selected Retirement Age","Count of Policies"]</t>
   </si>
   <si>
-    <t>Category selected retirement age data</t>
-  </si>
-  <si>
-    <t>["Main Plan Salaried","65","845","Main Plan Salaried DB----DC","65","191","Main Plan Deferred","65","81","DB/DC Deferred Members Main Plan","65","70","Main Weekly Paid DB/DC","65","69","Main Weekly Paid","65","57","DB AVC Deferred Member","65","5","DB AVC Member","65","3"]</t>
-  </si>
-  <si>
-    <t>["Main Plan Salaried","65","845","Main Plan Salaried DB/DC","65","191","Main Plan Deferred","65","81","DB/DC Deferred Members Main Plan","65","70","Main Weekly Paid DB/DC","65","69","Main Weekly Paid","65","57","DB AVC Deferred Member","65","5","DB AVC Member","65","3"]</t>
-  </si>
-  <si>
-    <t>YOUR M &amp; S PENSION SAVING PLAN</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>64%</t>
-  </si>
-  <si>
-    <t>THE TESCO RETIREMENT SAVINGS PLAN</t>
-  </si>
-  <si>
-    <t>8,873</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>["14,594","11,696","3,486","1,560","1,552","0"]</t>
-  </si>
-  <si>
-    <t>["TOTAL CALLS RECEIVED","32,888"]</t>
-  </si>
-  <si>
-    <t>RBS GROUP RETIREMENT SAVINGS PLAN (GIB)</t>
-  </si>
-  <si>
-    <t>SERCO</t>
-  </si>
-  <si>
-    <t>RBS GROUP RETIREMENT SAVINGS PLAN</t>
-  </si>
-  <si>
-    <t>1,884</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>["5,232","1,040","921","724","464","0"]</t>
-  </si>
-  <si>
-    <t>["TOTAL CALLS RECEIVED","8,381"]</t>
-  </si>
-  <si>
-    <t>SIEMENS HEALTHINEERS PENSION PLAN</t>
-  </si>
-  <si>
-    <t>SAINSBURY'S RETIREMENT SAVINGS PLAN</t>
-  </si>
-  <si>
-    <t>Tolerance</t>
-  </si>
-  <si>
-    <t>["New Members","65","204,554","Ex Stakeholder &amp; SIPP Members","65","26,641","Income Drawdown Category","65","6"]</t>
-  </si>
-  <si>
-    <t>New Members</t>
-  </si>
-  <si>
-    <t>Ex stakeholders &amp; SIPP Members</t>
-  </si>
-  <si>
-    <t>Drawdown category</t>
+    <t>["New Members","65","205,341","Ex Stakeholder &amp; SIPP Members","65","26,613","Income Drawdown Category","65","6"]</t>
+  </si>
+  <si>
+    <t>["New Members","65","205,206","Ex Stakeholder &amp; SIPP Members","65","26,583","Income Drawdown Category","65","6"]</t>
   </si>
   <si>
     <t>SAINSBURY'S SIPP</t>
@@ -229,47 +313,20 @@
     <t>ALLIANCE HEALTHCARE AND BOOTS RETIREMENT SAVINGS PLAN</t>
   </si>
   <si>
-    <t>GF61865001 - YOUR SODEXO RETIREMENT PLAN</t>
-  </si>
-  <si>
-    <t>["Sodexo Ltd - Monthly Paid","65","17,244","Sodexo Ltd - AE Weekly Paid","65","5,527","Sodexo Ltd - AE Monthly Paid","65","358","Sodexo Motivation Solutions UK Ltd","65","221","Sodexo Global Services Ltd","65","83","TVF Weekly Paid","65","21","Sports Travel &amp; Hospitality Group Ltd","65","20","Sodexo Ltd - Four Weekly Paid","65","9","Sodexo Travel","65","0"]</t>
-  </si>
-  <si>
-    <t>Sodexo Ltd Monthly Paid - Count Of Policies</t>
-  </si>
-  <si>
-    <t>Sodexo Ltd AE Weekly Paid - Count Of Policies</t>
-  </si>
-  <si>
-    <t>Sodexo Ltd AE Monthly Paid - Count Of Policies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sodexo Motivation Solutions UK Ltd               </t>
-  </si>
-  <si>
-    <t>Sodexo Global Services Ltd</t>
-  </si>
-  <si>
-    <t>TVF Weekly Paid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sports Travel &amp; Hospitality Group Ltd                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sodexo Ltd - Four Weekly Paid                               </t>
-  </si>
-  <si>
-    <t>Sodexo Travel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TVF Four weekly Temporary                                   </t>
+    <t>["Sodexo Ltd - Monthly Paid","65","17,229","Sodexo Ltd - AE Weekly Paid","65","4,910","Sodexo Ltd - AE Monthly Paid","65","358","Sodexo Motivation Solutions UK Ltd","65","221","Sodexo Global Services Ltd","65","83","TVF Weekly Paid","65","21","Sports Travel &amp; Hospitality Group Ltd","65","20","Sodexo Ltd - Four Weekly Paid","65","9","Sodexo Travel","65","0"]</t>
+  </si>
+  <si>
+    <t>["Sodexo Ltd - Monthly Paid","65","17,230","Sodexo Ltd - AE Weekly Paid","65","4,858","Sodexo Ltd - AE Monthly Paid","65","359","Sodexo Motivation Solutions UK Ltd","65","221","Sodexo Global Services Ltd","65","83","TVF Weekly Paid","65","21","Sports Travel &amp; Hospitality Group Ltd","65","20","Sodexo Ltd - Four Weekly Paid","65","9","Sodexo Travel","65","0"]</t>
+  </si>
+  <si>
+    <t>["New Members","65","208,975","Ex Stakeholder &amp; SIPP Members","65","26,283","Income Drawdown Category","65","6"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,8 +336,21 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -298,12 +368,42 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -315,9 +415,37 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -339,37 +467,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -385,15 +487,15 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -436,53 +538,146 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1179,108 +1374,403 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <f>IF(B3=C3,"PASS","FAIL")</f>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="127.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f>IF(B2=B3,"PASS","FAIL")</f>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="str">
-        <f>IF(B4=C4,"PASS","FAIL")</f>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f>IF(B3=B4,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="7">
+        <v>17494</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E17" s="9" t="str">
+        <f t="shared" ref="E17:E26" si="0">IF(AND((B17+(B17*D17))&gt;=C17,(B17-(B17*D17))&lt;=C17),"PASS","FAIL")</f>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7">
+        <v>4005</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="24">
+        <v>342</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="24">
+        <v>216</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="24">
+        <v>82</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="24">
+        <v>21</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="24">
+        <v>18</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="24">
+        <v>9</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="24">
+        <v>0</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="24">
+        <v>0</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:D8">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+  <conditionalFormatting sqref="E3:E4">
+    <cfRule type="cellIs" dxfId="67" priority="6" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
-    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
+  <conditionalFormatting sqref="E3:E4">
+    <cfRule type="cellIs" dxfId="66" priority="5" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E14">
+    <cfRule type="cellIs" dxfId="65" priority="4" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E14">
+    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E26">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E26">
+    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1299,73 +1789,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1401,73 +1891,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1503,73 +1993,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1605,73 +2095,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1707,73 +2197,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1809,73 +2299,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1911,73 +2401,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2013,71 +2503,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2113,73 +2603,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2215,76 +2705,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="10" t="str">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="16" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2307,99 +2797,290 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="27" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f>IF(B2=B3,"PASS","FAIL")</f>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f>IF(B3=B4,"PASS","FAIL")</f>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="str">
-        <f>IF(B3=C3,"PASS","FAIL")</f>
+      <c r="B5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="6" t="e">
+        <f t="shared" ref="E5" si="0">IF(AND((B5+(B5*D5))&gt;=C5,(B5-(B5*D5))&lt;=C5),"PASS","FAIL")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="28">
+        <v>208975</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f t="shared" ref="E17:E19" si="1">IF(AND((B17+(B17*D17))&gt;=C17,(B17-(B17*D17))&lt;=C17),"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="28">
+        <v>26283</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="31">
         <v>6</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="10" t="str">
-        <f>IF(B4=C4,"PASS","FAIL")</f>
+      <c r="C19" s="31"/>
+      <c r="D19" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E19" s="6" t="str">
+        <f t="shared" si="1"/>
         <v>FAIL</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:D8">
+  <conditionalFormatting sqref="E17:E19">
+    <cfRule type="cellIs" dxfId="61" priority="6" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E19">
+    <cfRule type="cellIs" dxfId="60" priority="5" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E4">
+    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E4">
+    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E14">
     <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
+  <conditionalFormatting sqref="E5:E14">
     <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -2424,73 +3105,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2526,77 +3207,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2632,73 +3313,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2734,73 +3415,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="19" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2836,73 +3517,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2938,73 +3619,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3041,73 +3722,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3143,73 +3824,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="23" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3272,81 +3953,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3449,9 +4130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C14"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3462,216 +4141,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="17">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="str">
+      <c r="E3" s="4" t="str">
         <f>IF(B2=B3,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="17">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="str">
+      <c r="E4" s="4" t="str">
         <f>IF(B3=B4,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="19">
-        <v>17244</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="11">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="18">
+        <v>17229</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="8">
         <v>0.05</v>
       </c>
-      <c r="E5" s="5" t="str">
+      <c r="E5" s="9" t="str">
         <f t="shared" ref="E5:E14" si="0">IF(AND((B5+(B5*D5))&gt;=C5,(B5-(B5*D5))&lt;=C5),"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="19">
-        <v>5527</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="11">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="18">
+        <v>4910</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="8">
         <v>0.05</v>
       </c>
-      <c r="E6" s="5" t="str">
+      <c r="E6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="18">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
         <v>358</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>0.05</v>
       </c>
-      <c r="E7" s="5" t="str">
+      <c r="E7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="18">
+      <c r="A8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
         <v>221</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>0.05</v>
       </c>
-      <c r="E8" s="5" t="str">
+      <c r="E8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="18">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
         <v>83</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>0.05</v>
       </c>
-      <c r="E9" s="5" t="str">
+      <c r="E9" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="18">
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
         <v>21</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>0.05</v>
       </c>
-      <c r="E10" s="5" t="str">
+      <c r="E10" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="18">
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
         <v>20</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>0.05</v>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="18">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>0.05</v>
       </c>
-      <c r="E12" s="5" t="str">
+      <c r="E12" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="18">
+      <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <v>0.05</v>
       </c>
-      <c r="E13" s="5" t="str">
+      <c r="E13" s="9" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="18">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>0.05</v>
       </c>
-      <c r="E14" s="5" t="str">
+      <c r="E14" s="9" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
@@ -3734,73 +4410,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3837,73 +4513,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3939,81 +4615,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4049,73 +4725,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4140,9 +4816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4152,101 +4826,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="11">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="8">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="str">
+      <c r="E3" s="4" t="str">
         <f>IF(B2=B3,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+      <c r="A4" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="11">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="str">
+      <c r="E4" s="4" t="str">
         <f>IF(B3=B4,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="19">
-        <v>204554</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="11">
+      <c r="A5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="18">
+        <v>205341</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="8">
         <v>0.05</v>
       </c>
-      <c r="E5" s="5" t="str">
+      <c r="E5" s="9" t="str">
         <f t="shared" ref="E5:E7" si="0">IF(AND((B5+(B5*D5))&gt;=C5,(B5-(B5*D5))&lt;=C5),"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="19">
-        <v>26641</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="11">
+      <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="18">
+        <v>26613</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="8">
         <v>0.05</v>
       </c>
-      <c r="E6" s="5" t="str">
+      <c r="E6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="18">
+      <c r="A7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>0.05</v>
       </c>
-      <c r="E7" s="5" t="str">
+      <c r="E7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>FAIL</v>
       </c>
@@ -4296,73 +4975,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="9" t="str">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="15" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10" t="str">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="16" t="str">
         <f>IF(B4=C4,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10" t="str">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="16" t="str">
         <f t="shared" ref="D5:D6" si="0">IF(B5=C5,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="str">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>